<commit_message>
Despues de reseteo por id. Fin ruta 1. Antes de fortaleza team rocket.
</commit_message>
<xml_diff>
--- a/PokemonUsados.xlsx
+++ b/PokemonUsados.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alejandro Sanchez\Desktop\SupremeLeague\Pokemon_Liga_Suprema\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3845A519-AFAE-4872-A7FA-125E206C6C4C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D180BC5-DA62-414D-B128-6E93684D75DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Information" sheetId="1" r:id="rId1"/>
@@ -3657,6 +3657,9 @@
     <xf numFmtId="0" fontId="21" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -3683,9 +3686,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -4036,178 +4036,178 @@
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="45" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="41"/>
-      <c r="C1" s="41"/>
-      <c r="D1" s="41"/>
-      <c r="E1" s="41"/>
-      <c r="F1" s="41"/>
-      <c r="G1" s="41"/>
-      <c r="H1" s="41"/>
-      <c r="I1" s="41"/>
-      <c r="J1" s="41"/>
-      <c r="K1" s="41"/>
+      <c r="A1" s="46" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="42"/>
+      <c r="C1" s="42"/>
+      <c r="D1" s="42"/>
+      <c r="E1" s="42"/>
+      <c r="F1" s="42"/>
+      <c r="G1" s="42"/>
+      <c r="H1" s="42"/>
+      <c r="I1" s="42"/>
+      <c r="J1" s="42"/>
+      <c r="K1" s="42"/>
     </row>
     <row r="2" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="40" t="s">
+      <c r="A2" s="41" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="41"/>
-      <c r="C2" s="41"/>
-      <c r="D2" s="41"/>
-      <c r="E2" s="41"/>
-      <c r="F2" s="41"/>
-      <c r="G2" s="41"/>
-      <c r="H2" s="41"/>
-      <c r="I2" s="41"/>
-      <c r="J2" s="41"/>
-      <c r="K2" s="41"/>
+      <c r="B2" s="42"/>
+      <c r="C2" s="42"/>
+      <c r="D2" s="42"/>
+      <c r="E2" s="42"/>
+      <c r="F2" s="42"/>
+      <c r="G2" s="42"/>
+      <c r="H2" s="42"/>
+      <c r="I2" s="42"/>
+      <c r="J2" s="42"/>
+      <c r="K2" s="42"/>
     </row>
     <row r="3" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="40" t="s">
+      <c r="A3" s="41" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="41"/>
-      <c r="C3" s="41"/>
-      <c r="D3" s="41"/>
-      <c r="E3" s="41"/>
-      <c r="F3" s="41"/>
-      <c r="G3" s="41"/>
-      <c r="H3" s="41"/>
-      <c r="I3" s="41"/>
-      <c r="J3" s="41"/>
-      <c r="K3" s="41"/>
+      <c r="B3" s="42"/>
+      <c r="C3" s="42"/>
+      <c r="D3" s="42"/>
+      <c r="E3" s="42"/>
+      <c r="F3" s="42"/>
+      <c r="G3" s="42"/>
+      <c r="H3" s="42"/>
+      <c r="I3" s="42"/>
+      <c r="J3" s="42"/>
+      <c r="K3" s="42"/>
     </row>
     <row r="4" spans="1:11" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A4" s="40"/>
-      <c r="B4" s="41"/>
-      <c r="C4" s="41"/>
-      <c r="D4" s="41"/>
-      <c r="E4" s="41"/>
-      <c r="F4" s="41"/>
-      <c r="G4" s="41"/>
-      <c r="H4" s="41"/>
-      <c r="I4" s="41"/>
-      <c r="J4" s="41"/>
-      <c r="K4" s="41"/>
+      <c r="A4" s="41"/>
+      <c r="B4" s="42"/>
+      <c r="C4" s="42"/>
+      <c r="D4" s="42"/>
+      <c r="E4" s="42"/>
+      <c r="F4" s="42"/>
+      <c r="G4" s="42"/>
+      <c r="H4" s="42"/>
+      <c r="I4" s="42"/>
+      <c r="J4" s="42"/>
+      <c r="K4" s="42"/>
     </row>
     <row r="5" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="41"/>
-      <c r="B5" s="41"/>
-      <c r="C5" s="41"/>
-      <c r="D5" s="41"/>
-      <c r="E5" s="41"/>
-      <c r="F5" s="41"/>
-      <c r="G5" s="41"/>
-      <c r="H5" s="41"/>
-      <c r="I5" s="41"/>
-      <c r="J5" s="41"/>
-      <c r="K5" s="41"/>
+      <c r="A5" s="42"/>
+      <c r="B5" s="42"/>
+      <c r="C5" s="42"/>
+      <c r="D5" s="42"/>
+      <c r="E5" s="42"/>
+      <c r="F5" s="42"/>
+      <c r="G5" s="42"/>
+      <c r="H5" s="42"/>
+      <c r="I5" s="42"/>
+      <c r="J5" s="42"/>
+      <c r="K5" s="42"/>
     </row>
     <row r="6" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="46" t="s">
+      <c r="A6" s="47" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="41"/>
-      <c r="C6" s="41"/>
-      <c r="D6" s="41"/>
-      <c r="E6" s="41"/>
-      <c r="F6" s="41"/>
-      <c r="G6" s="41"/>
-      <c r="H6" s="41"/>
-      <c r="I6" s="41"/>
-      <c r="J6" s="41"/>
-      <c r="K6" s="41"/>
+      <c r="B6" s="42"/>
+      <c r="C6" s="42"/>
+      <c r="D6" s="42"/>
+      <c r="E6" s="42"/>
+      <c r="F6" s="42"/>
+      <c r="G6" s="42"/>
+      <c r="H6" s="42"/>
+      <c r="I6" s="42"/>
+      <c r="J6" s="42"/>
+      <c r="K6" s="42"/>
     </row>
     <row r="7" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="47" t="s">
+      <c r="A7" s="48" t="s">
         <v>4</v>
       </c>
-      <c r="B7" s="41"/>
-      <c r="C7" s="41"/>
-      <c r="D7" s="41"/>
-      <c r="E7" s="41"/>
-      <c r="F7" s="41"/>
-      <c r="G7" s="41"/>
-      <c r="H7" s="41"/>
-      <c r="I7" s="41"/>
-      <c r="J7" s="41"/>
-      <c r="K7" s="41"/>
+      <c r="B7" s="42"/>
+      <c r="C7" s="42"/>
+      <c r="D7" s="42"/>
+      <c r="E7" s="42"/>
+      <c r="F7" s="42"/>
+      <c r="G7" s="42"/>
+      <c r="H7" s="42"/>
+      <c r="I7" s="42"/>
+      <c r="J7" s="42"/>
+      <c r="K7" s="42"/>
     </row>
     <row r="8" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="48" t="s">
+      <c r="A8" s="49" t="s">
         <v>5</v>
       </c>
-      <c r="B8" s="41"/>
-      <c r="C8" s="41"/>
-      <c r="D8" s="41"/>
-      <c r="E8" s="41"/>
-      <c r="F8" s="41"/>
-      <c r="G8" s="41"/>
-      <c r="H8" s="41"/>
-      <c r="I8" s="41"/>
-      <c r="J8" s="41"/>
-      <c r="K8" s="41"/>
+      <c r="B8" s="42"/>
+      <c r="C8" s="42"/>
+      <c r="D8" s="42"/>
+      <c r="E8" s="42"/>
+      <c r="F8" s="42"/>
+      <c r="G8" s="42"/>
+      <c r="H8" s="42"/>
+      <c r="I8" s="42"/>
+      <c r="J8" s="42"/>
+      <c r="K8" s="42"/>
     </row>
     <row r="9" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="49" t="s">
+      <c r="A9" s="50" t="s">
         <v>6</v>
       </c>
-      <c r="B9" s="41"/>
-      <c r="C9" s="41"/>
-      <c r="D9" s="41"/>
-      <c r="E9" s="41"/>
-      <c r="F9" s="41"/>
-      <c r="G9" s="41"/>
-      <c r="H9" s="41"/>
-      <c r="I9" s="41"/>
-      <c r="J9" s="41"/>
-      <c r="K9" s="41"/>
+      <c r="B9" s="42"/>
+      <c r="C9" s="42"/>
+      <c r="D9" s="42"/>
+      <c r="E9" s="42"/>
+      <c r="F9" s="42"/>
+      <c r="G9" s="42"/>
+      <c r="H9" s="42"/>
+      <c r="I9" s="42"/>
+      <c r="J9" s="42"/>
+      <c r="K9" s="42"/>
     </row>
     <row r="10" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="40"/>
-      <c r="B10" s="41"/>
-      <c r="C10" s="41"/>
-      <c r="D10" s="41"/>
-      <c r="E10" s="41"/>
-      <c r="F10" s="41"/>
-      <c r="G10" s="41"/>
-      <c r="H10" s="41"/>
-      <c r="I10" s="41"/>
-      <c r="J10" s="41"/>
-      <c r="K10" s="41"/>
+      <c r="A10" s="41"/>
+      <c r="B10" s="42"/>
+      <c r="C10" s="42"/>
+      <c r="D10" s="42"/>
+      <c r="E10" s="42"/>
+      <c r="F10" s="42"/>
+      <c r="G10" s="42"/>
+      <c r="H10" s="42"/>
+      <c r="I10" s="42"/>
+      <c r="J10" s="42"/>
+      <c r="K10" s="42"/>
     </row>
     <row r="11" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="42" t="s">
+      <c r="A11" s="43" t="s">
         <v>7</v>
       </c>
-      <c r="B11" s="41"/>
-      <c r="C11" s="41"/>
-      <c r="D11" s="41"/>
-      <c r="E11" s="41"/>
-      <c r="F11" s="41"/>
-      <c r="G11" s="41"/>
-      <c r="H11" s="41"/>
-      <c r="I11" s="41"/>
-      <c r="J11" s="41"/>
-      <c r="K11" s="41"/>
+      <c r="B11" s="42"/>
+      <c r="C11" s="42"/>
+      <c r="D11" s="42"/>
+      <c r="E11" s="42"/>
+      <c r="F11" s="42"/>
+      <c r="G11" s="42"/>
+      <c r="H11" s="42"/>
+      <c r="I11" s="42"/>
+      <c r="J11" s="42"/>
+      <c r="K11" s="42"/>
     </row>
     <row r="12" spans="1:11" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A12" s="43" t="s">
+      <c r="A12" s="44" t="s">
         <v>8</v>
       </c>
-      <c r="B12" s="41"/>
-      <c r="C12" s="41"/>
-      <c r="D12" s="41"/>
-      <c r="E12" s="41"/>
-      <c r="F12" s="41"/>
-      <c r="G12" s="41"/>
-      <c r="H12" s="41"/>
-      <c r="I12" s="41"/>
-      <c r="J12" s="41"/>
-      <c r="K12" s="41"/>
+      <c r="B12" s="42"/>
+      <c r="C12" s="42"/>
+      <c r="D12" s="42"/>
+      <c r="E12" s="42"/>
+      <c r="F12" s="42"/>
+      <c r="G12" s="42"/>
+      <c r="H12" s="42"/>
+      <c r="I12" s="42"/>
+      <c r="J12" s="42"/>
+      <c r="K12" s="42"/>
     </row>
     <row r="13" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="1"/>
@@ -4219,19 +4219,19 @@
       <c r="G13" s="1"/>
     </row>
     <row r="14" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="44" t="s">
+      <c r="A14" s="45" t="s">
         <v>9</v>
       </c>
-      <c r="B14" s="41"/>
-      <c r="C14" s="41"/>
-      <c r="D14" s="41"/>
-      <c r="E14" s="41"/>
-      <c r="F14" s="41"/>
-      <c r="G14" s="41"/>
-      <c r="H14" s="41"/>
-      <c r="I14" s="41"/>
-      <c r="J14" s="41"/>
-      <c r="K14" s="41"/>
+      <c r="B14" s="42"/>
+      <c r="C14" s="42"/>
+      <c r="D14" s="42"/>
+      <c r="E14" s="42"/>
+      <c r="F14" s="42"/>
+      <c r="G14" s="42"/>
+      <c r="H14" s="42"/>
+      <c r="I14" s="42"/>
+      <c r="J14" s="42"/>
+      <c r="K14" s="42"/>
     </row>
   </sheetData>
   <mergeCells count="12">
@@ -4259,8 +4259,8 @@
   </sheetPr>
   <dimension ref="A1:AB152"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A117" workbookViewId="0">
-      <selection activeCell="K139" sqref="K139"/>
+    <sheetView tabSelected="1" topLeftCell="A54" workbookViewId="0">
+      <selection activeCell="T86" sqref="T86"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -4630,7 +4630,7 @@
       <c r="W4" s="35" t="s">
         <v>1041</v>
       </c>
-      <c r="X4" s="50" t="s">
+      <c r="X4" s="40" t="s">
         <v>1042</v>
       </c>
       <c r="Y4" s="14">
@@ -4881,7 +4881,7 @@
         <v>50</v>
       </c>
       <c r="O7" s="35" t="s">
-        <v>1041</v>
+        <v>1042</v>
       </c>
       <c r="P7" s="13" t="s">
         <v>1041</v>
@@ -5150,7 +5150,7 @@
         <v>1041</v>
       </c>
       <c r="L10" s="13" t="s">
-        <v>1041</v>
+        <v>1042</v>
       </c>
       <c r="M10" s="10">
         <f t="shared" si="3"/>
@@ -5216,7 +5216,7 @@
       <c r="C11" s="35" t="s">
         <v>1042</v>
       </c>
-      <c r="D11" s="50" t="s">
+      <c r="D11" s="40" t="s">
         <v>1042</v>
       </c>
       <c r="E11" s="15">
@@ -5309,7 +5309,7 @@
       <c r="C12" s="37" t="s">
         <v>1041</v>
       </c>
-      <c r="D12" s="50" t="s">
+      <c r="D12" s="40" t="s">
         <v>1042</v>
       </c>
       <c r="E12" s="15">
@@ -5495,7 +5495,7 @@
       <c r="C14" s="37" t="s">
         <v>1042</v>
       </c>
-      <c r="D14" s="50" t="s">
+      <c r="D14" s="40" t="s">
         <v>1042</v>
       </c>
       <c r="E14" s="15">
@@ -5588,7 +5588,7 @@
       <c r="C15" s="37" t="s">
         <v>1041</v>
       </c>
-      <c r="D15" s="50" t="s">
+      <c r="D15" s="40" t="s">
         <v>1042</v>
       </c>
       <c r="E15" s="15">
@@ -5930,7 +5930,7 @@
         <v>129</v>
       </c>
       <c r="W18" s="35" t="s">
-        <v>1041</v>
+        <v>1042</v>
       </c>
       <c r="X18" s="13" t="s">
         <v>1041</v>
@@ -6343,7 +6343,7 @@
         <v>160</v>
       </c>
       <c r="G23" s="35" t="s">
-        <v>1041</v>
+        <v>1042</v>
       </c>
       <c r="H23" s="13" t="s">
         <v>1041</v>
@@ -6436,7 +6436,7 @@
         <v>167</v>
       </c>
       <c r="G24" s="35" t="s">
-        <v>1041</v>
+        <v>1042</v>
       </c>
       <c r="H24" s="13" t="s">
         <v>1041</v>
@@ -6529,7 +6529,7 @@
         <v>174</v>
       </c>
       <c r="G25" s="35" t="s">
-        <v>1041</v>
+        <v>1042</v>
       </c>
       <c r="H25" s="13" t="s">
         <v>1041</v>
@@ -6981,7 +6981,7 @@
         <v>208</v>
       </c>
       <c r="C30" s="35" t="s">
-        <v>1041</v>
+        <v>1042</v>
       </c>
       <c r="D30" s="13" t="s">
         <v>1041</v>
@@ -7260,7 +7260,7 @@
         <v>229</v>
       </c>
       <c r="C33" s="35" t="s">
-        <v>1041</v>
+        <v>1042</v>
       </c>
       <c r="D33" s="13" t="s">
         <v>1041</v>
@@ -8296,7 +8296,7 @@
         <v>307</v>
       </c>
       <c r="G44" s="35" t="s">
-        <v>1041</v>
+        <v>1042</v>
       </c>
       <c r="H44" s="13" t="s">
         <v>1041</v>
@@ -8392,7 +8392,7 @@
         <v>1041</v>
       </c>
       <c r="H45" s="13" t="s">
-        <v>1041</v>
+        <v>1042</v>
       </c>
       <c r="I45" s="9">
         <f t="shared" si="2"/>
@@ -9531,7 +9531,7 @@
         <v>400</v>
       </c>
       <c r="O57" s="35" t="s">
-        <v>1041</v>
+        <v>1042</v>
       </c>
       <c r="P57" s="13" t="s">
         <v>1041</v>
@@ -9823,7 +9823,7 @@
         <v>422</v>
       </c>
       <c r="S60" s="35" t="s">
-        <v>1041</v>
+        <v>1042</v>
       </c>
       <c r="T60" s="13" t="s">
         <v>1042</v>
@@ -9867,7 +9867,7 @@
         <v>1041</v>
       </c>
       <c r="D61" s="13" t="s">
-        <v>1041</v>
+        <v>1042</v>
       </c>
       <c r="E61" s="15">
         <f t="shared" si="1"/>
@@ -10290,7 +10290,7 @@
       <c r="S65" s="35" t="s">
         <v>1042</v>
       </c>
-      <c r="T65" s="50" t="s">
+      <c r="T65" s="40" t="s">
         <v>1042</v>
       </c>
       <c r="U65" s="19">
@@ -10383,7 +10383,7 @@
       <c r="S66" s="35" t="s">
         <v>1041</v>
       </c>
-      <c r="T66" s="50" t="s">
+      <c r="T66" s="40" t="s">
         <v>1042</v>
       </c>
       <c r="U66" s="19">
@@ -10554,7 +10554,7 @@
         <v>477</v>
       </c>
       <c r="O68" s="35" t="s">
-        <v>1041</v>
+        <v>1042</v>
       </c>
       <c r="P68" s="13" t="s">
         <v>1041</v>
@@ -10740,7 +10740,7 @@
         <v>491</v>
       </c>
       <c r="O70" s="35" t="s">
-        <v>1041</v>
+        <v>1042</v>
       </c>
       <c r="P70" s="13" t="s">
         <v>1041</v>
@@ -10952,7 +10952,7 @@
         <v>507</v>
       </c>
       <c r="W72" s="35" t="s">
-        <v>1041</v>
+        <v>1042</v>
       </c>
       <c r="X72" s="13" t="s">
         <v>1041</v>
@@ -11497,7 +11497,7 @@
         <v>548</v>
       </c>
       <c r="S78" s="35" t="s">
-        <v>1041</v>
+        <v>1042</v>
       </c>
       <c r="T78" s="13" t="s">
         <v>1041</v>
@@ -11856,7 +11856,7 @@
         <v>575</v>
       </c>
       <c r="O82" s="35" t="s">
-        <v>1041</v>
+        <v>1042</v>
       </c>
       <c r="P82" s="13" t="s">
         <v>1041</v>
@@ -12151,7 +12151,7 @@
         <v>1041</v>
       </c>
       <c r="T85" s="13" t="s">
-        <v>1041</v>
+        <v>1042</v>
       </c>
       <c r="U85" s="19">
         <f t="shared" si="5"/>
@@ -12204,7 +12204,7 @@
       <c r="G86" s="35" t="s">
         <v>1041</v>
       </c>
-      <c r="H86" s="50" t="s">
+      <c r="H86" s="40" t="s">
         <v>1042</v>
       </c>
       <c r="I86" s="9">
@@ -12895,7 +12895,7 @@
         <v>1041</v>
       </c>
       <c r="T93" s="13" t="s">
-        <v>1041</v>
+        <v>1042</v>
       </c>
       <c r="U93" s="19">
         <f t="shared" si="5"/>
@@ -12974,7 +12974,7 @@
       <c r="O94" s="35" t="s">
         <v>1042</v>
       </c>
-      <c r="P94" s="50" t="s">
+      <c r="P94" s="40" t="s">
         <v>1042</v>
       </c>
       <c r="Q94" s="18">
@@ -13277,7 +13277,7 @@
         <v>682</v>
       </c>
       <c r="W97" s="35" t="s">
-        <v>1041</v>
+        <v>1042</v>
       </c>
       <c r="X97" s="13" t="s">
         <v>1041</v>
@@ -13889,7 +13889,7 @@
         <v>728</v>
       </c>
       <c r="K104" s="35" t="s">
-        <v>1041</v>
+        <v>1042</v>
       </c>
       <c r="L104" s="13" t="s">
         <v>1041</v>
@@ -14170,7 +14170,7 @@
       <c r="K107" s="35" t="s">
         <v>1041</v>
       </c>
-      <c r="L107" s="50" t="s">
+      <c r="L107" s="40" t="s">
         <v>1042</v>
       </c>
       <c r="M107" s="11">
@@ -14207,7 +14207,7 @@
         <v>752</v>
       </c>
       <c r="W107" s="35" t="s">
-        <v>1041</v>
+        <v>1042</v>
       </c>
       <c r="X107" s="13" t="s">
         <v>1041</v>
@@ -15007,7 +15007,7 @@
       <c r="K116" s="35" t="s">
         <v>1041</v>
       </c>
-      <c r="L116" s="50" t="s">
+      <c r="L116" s="40" t="s">
         <v>1042</v>
       </c>
       <c r="M116" s="11">
@@ -15072,7 +15072,7 @@
         <v>817</v>
       </c>
       <c r="C117" s="35" t="s">
-        <v>1041</v>
+        <v>1042</v>
       </c>
       <c r="D117" s="13" t="s">
         <v>1041</v>
@@ -15100,7 +15100,7 @@
       <c r="K117" s="35" t="s">
         <v>1041</v>
       </c>
-      <c r="L117" s="50" t="s">
+      <c r="L117" s="40" t="s">
         <v>1041</v>
       </c>
       <c r="M117" s="11">
@@ -15287,7 +15287,7 @@
         <v>1041</v>
       </c>
       <c r="L119" s="13" t="s">
-        <v>1041</v>
+        <v>1042</v>
       </c>
       <c r="M119" s="11">
         <f t="shared" si="3"/>
@@ -15460,7 +15460,7 @@
         <v>1041</v>
       </c>
       <c r="H121" s="13" t="s">
-        <v>1041</v>
+        <v>1042</v>
       </c>
       <c r="I121" s="10">
         <f t="shared" si="2"/>
@@ -15483,7 +15483,7 @@
         <v>848</v>
       </c>
       <c r="O121" s="35" t="s">
-        <v>1041</v>
+        <v>1042</v>
       </c>
       <c r="P121" s="13" t="s">
         <v>1041</v>
@@ -15669,7 +15669,7 @@
         <v>862</v>
       </c>
       <c r="O123" s="35" t="s">
-        <v>1041</v>
+        <v>1042</v>
       </c>
       <c r="P123" s="13" t="s">
         <v>1041</v>
@@ -16015,7 +16015,7 @@
         <v>888</v>
       </c>
       <c r="G127" s="35" t="s">
-        <v>1041</v>
+        <v>1042</v>
       </c>
       <c r="H127" s="13" t="s">
         <v>1041</v>
@@ -16245,7 +16245,6 @@
         <v>905</v>
       </c>
       <c r="AA129" s="8" cm="1">
-        <f t="array" ref="AA129">COUNTIF(G2:G151,'TRUE')+COUNTIF(C2:C151,'TRUE')+COUNTIF(K2:K151,'TRUE')+COUNTIF(O2:O151,'TRUE')+COUNTIF(S2:S151,'TRUE')+COUNTIF(W2:W151,'TRUE')</f>
         <v>0</v>
       </c>
       <c r="AB129" s="8">
@@ -16462,7 +16461,7 @@
         <v>921</v>
       </c>
       <c r="K132" s="35" t="s">
-        <v>1041</v>
+        <v>1042</v>
       </c>
       <c r="L132" s="13" t="s">
         <v>1041</v>
@@ -16617,7 +16616,7 @@
         <v>932</v>
       </c>
       <c r="G134" s="35" t="s">
-        <v>1041</v>
+        <v>1042</v>
       </c>
       <c r="H134" s="13" t="s">
         <v>1041</v>
@@ -16740,7 +16739,7 @@
         <v>941</v>
       </c>
       <c r="S135" s="35" t="s">
-        <v>1041</v>
+        <v>1042</v>
       </c>
       <c r="T135" s="13" t="s">
         <v>1041</v>
@@ -17574,7 +17573,7 @@
         <v>1001</v>
       </c>
       <c r="S145" s="35" t="s">
-        <v>1041</v>
+        <v>1042</v>
       </c>
       <c r="T145" s="13" t="s">
         <v>1041</v>
@@ -17648,7 +17647,7 @@
         <v>1041</v>
       </c>
       <c r="P146" s="13" t="s">
-        <v>1041</v>
+        <v>1042</v>
       </c>
       <c r="Q146" s="20">
         <f t="shared" si="4"/>
@@ -17871,7 +17870,7 @@
         <v>1022</v>
       </c>
       <c r="G149" s="35" t="s">
-        <v>1041</v>
+        <v>1042</v>
       </c>
       <c r="H149" s="13" t="s">
         <v>1041</v>

</xml_diff>

<commit_message>
Justo antes de entregar medalla al jugador (Combate contra Gladio Ya hecho). A falta de entrega chula de medallas
</commit_message>
<xml_diff>
--- a/PokemonUsados.xlsx
+++ b/PokemonUsados.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alejandro Sanchez\Desktop\SupremeLeague\Pokemon_Liga_Suprema\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D180BC5-DA62-414D-B128-6E93684D75DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2AC358F4-2AF3-42FC-AA3A-44B1387D48C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -4259,8 +4259,8 @@
   </sheetPr>
   <dimension ref="A1:AB152"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A54" workbookViewId="0">
-      <selection activeCell="T86" sqref="T86"/>
+    <sheetView tabSelected="1" topLeftCell="B100" workbookViewId="0">
+      <selection activeCell="T146" sqref="T146"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -4445,7 +4445,7 @@
         <v>1042</v>
       </c>
       <c r="X2" s="33" t="s">
-        <v>1041</v>
+        <v>1042</v>
       </c>
       <c r="Y2" s="14">
         <f>U151+1</f>
@@ -5003,7 +5003,7 @@
         <v>1041</v>
       </c>
       <c r="X8" s="13" t="s">
-        <v>1041</v>
+        <v>1042</v>
       </c>
       <c r="Y8" s="16">
         <f t="shared" si="6"/>
@@ -5375,7 +5375,7 @@
         <v>1041</v>
       </c>
       <c r="X12" s="13" t="s">
-        <v>1041</v>
+        <v>1042</v>
       </c>
       <c r="Y12" s="16">
         <f t="shared" si="6"/>
@@ -6398,7 +6398,7 @@
         <v>1041</v>
       </c>
       <c r="X23" s="13" t="s">
-        <v>1041</v>
+        <v>1042</v>
       </c>
       <c r="Y23" s="16">
         <f t="shared" si="6"/>
@@ -16910,7 +16910,7 @@
         <v>1042</v>
       </c>
       <c r="T137" s="13" t="s">
-        <v>1041</v>
+        <v>1042</v>
       </c>
       <c r="U137" s="19">
         <f t="shared" si="5"/>
@@ -17156,7 +17156,7 @@
         <v>1041</v>
       </c>
       <c r="T140" s="13" t="s">
-        <v>1041</v>
+        <v>1042</v>
       </c>
       <c r="U140" s="19">
         <f t="shared" si="5"/>
@@ -17576,7 +17576,7 @@
         <v>1042</v>
       </c>
       <c r="T145" s="13" t="s">
-        <v>1041</v>
+        <v>1042</v>
       </c>
       <c r="U145" s="19">
         <f t="shared" si="5"/>
@@ -17828,7 +17828,7 @@
         <v>1041</v>
       </c>
       <c r="T148" s="13" t="s">
-        <v>1041</v>
+        <v>1042</v>
       </c>
       <c r="U148" s="19">
         <f t="shared" si="5"/>

</xml_diff>